<commit_message>
Out of stock list section
</commit_message>
<xml_diff>
--- a/public/uploads/stocks/stock_list_88.xlsx
+++ b/public/uploads/stocks/stock_list_88.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Documents\SametimeFileTransfers\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="25365" windowHeight="14595" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -60,16 +60,34 @@
     <t>Average Monthly Consumption (AMC) in Packs</t>
   </si>
   <si>
+    <t>tablets</t>
+  </si>
+  <si>
     <t>mg</t>
   </si>
   <si>
+    <t>64745</t>
+  </si>
+  <si>
+    <t>2017-03-10</t>
+  </si>
+  <si>
+    <t>EMS</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
     <t>Expiry Date (yyyy-mm-dd)</t>
   </si>
   <si>
-    <t>g487654</t>
-  </si>
-  <si>
-    <t>testing *8</t>
+    <t>Test 5th</t>
+  </si>
+  <si>
+    <t>Test 20th</t>
+  </si>
+  <si>
+    <t>64745sd</t>
   </si>
 </sst>
 </file>
@@ -470,24 +488,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="4" width="20" customWidth="1"/>
-    <col min="5" max="6" width="30" customWidth="1"/>
-    <col min="7" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="30" style="3" customWidth="1"/>
-    <col min="10" max="10" width="30" customWidth="1"/>
-    <col min="11" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="30" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,7 +520,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
@@ -535,41 +542,88 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
       </c>
       <c r="D2">
         <v>1000</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
       </c>
       <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="3">
-        <v>43831</v>
+      <c r="I2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
       </c>
       <c r="K2">
-        <v>1245</v>
+        <v>12</v>
       </c>
       <c r="L2">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="M2">
-        <v>10</v>
-      </c>
-      <c r="N2">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="4">
+        <v>12</v>
+      </c>
+      <c r="L3" s="4">
+        <v>24</v>
+      </c>
+      <c r="M3" s="4">
+        <v>12</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -589,6 +643,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>